<commit_message>
Updating simple excel file template
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yu021\PycharmProjects\ldr-utils-py\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jon/dev/git/ldrpyutils/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="registerinfo" sheetId="2" r:id="rId1"/>
     <sheet name="testreg" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -108,7 +111,7 @@
     <t>registry_location</t>
   </si>
   <si>
-    <t>http://registry.it.csiro.au/sandbox/csiro/test-bba/testreg1</t>
+    <t>http://registry.it.csiro.au/sandbox/csiro/utils/testreg1</t>
   </si>
 </sst>
 </file>
@@ -229,9 +232,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -264,9 +267,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -448,17 +451,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -466,7 +469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -474,7 +477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -482,7 +485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -490,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -511,21 +514,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,7 +547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -565,7 +567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -585,7 +587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updating simple excel template
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jon/dev/git/ldrpyutils/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\git\github\csiro-lw-ld\ldrpyutils\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="registerinfo" sheetId="2" r:id="rId1"/>
@@ -17,18 +17,219 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yu, Jonathan (L&amp;W, Clayton)</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Value of id is the name of the sheet with the items in them. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A short label to describe the register or container</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description or definition for the register or container</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Expect a URL for the location of the register online.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A description of the register's source material</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A person or organisation unit responsible for maintaining this register.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yu, Jonathan (L&amp;W, Clayton)</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This is the identifier for the item in this register</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A short label for the item</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A description or definition of the register item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>An abbreviation or technical/scientific notation for the item</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yu, Jonathan (L&amp;W, Clayton):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+A general note for users to be aware of.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Source of the item's definition.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Reference to a broader item in this register. Use the value in the 'id' column in this sheet.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>label</t>
   </si>
@@ -42,9 +243,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>definition</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -72,9 +270,6 @@
     <t>aaaa</t>
   </si>
   <si>
-    <t>aaaaaa</t>
-  </si>
-  <si>
     <t>bb</t>
   </si>
   <si>
@@ -84,9 +279,6 @@
     <t>bbbb</t>
   </si>
   <si>
-    <t>bbbbbb</t>
-  </si>
-  <si>
     <t>cc</t>
   </si>
   <si>
@@ -96,9 +288,6 @@
     <t>cccc</t>
   </si>
   <si>
-    <t>cccccc</t>
-  </si>
-  <si>
     <t>Register_property</t>
   </si>
   <si>
@@ -112,13 +301,22 @@
   </si>
   <si>
     <t>http://registry.it.csiro.au/sandbox/csiro/utils/testreg1</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>broader</t>
+  </si>
+  <si>
+    <t>maintainer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +339,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -448,57 +665,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -507,29 +734,30 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="17.83203125" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -544,70 +772,66 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring core library to handle revised single register template
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="registerinfo" sheetId="2" r:id="rId1"/>
-    <sheet name="testreg" sheetId="1" r:id="rId2"/>
+    <sheet name="testreg1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>label</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Register_property_value</t>
   </si>
   <si>
-    <t>testreg</t>
-  </si>
-  <si>
     <t>registry_location</t>
   </si>
   <si>
@@ -310,6 +307,24 @@
   </si>
   <si>
     <t>maintainer</t>
+  </si>
+  <si>
+    <t>Github repo at  https://github.com/CSIRO-LW-LD/ldrpyutils</t>
+  </si>
+  <si>
+    <t>Jonathan Yu</t>
+  </si>
+  <si>
+    <t>Green book</t>
+  </si>
+  <si>
+    <t>Red book</t>
+  </si>
+  <si>
+    <t>Yellow book</t>
+  </si>
+  <si>
+    <t>testreg1</t>
   </si>
 </sst>
 </file>
@@ -668,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -712,20 +727,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -742,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -794,6 +815,9 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -811,6 +835,12 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -827,6 +857,12 @@
       </c>
       <c r="E4" t="s">
         <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating single register template
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>label</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>testreg1</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Blue book</t>
   </si>
 </sst>
 </file>
@@ -761,10 +767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,6 +871,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated embedded documentation (comments)
and added another row to the table
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\git\github\csiro-lw-ld\ldrpyutils\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="1155" yWindow="0" windowWidth="13650" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="registerinfo" sheetId="2" r:id="rId1"/>
-    <sheet name="testreg1" sheetId="1" r:id="rId2"/>
+    <sheet name="testreg4" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -144,7 +144,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>A short label for the item</t>
+          <t>A short label for the item, aka the 'term' which this concept definition is about</t>
         </r>
       </text>
     </comment>
@@ -157,7 +157,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>A description or definition of the register item.</t>
+          <t>A description or definition of the item.</t>
         </r>
       </text>
     </comment>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>label</t>
   </si>
@@ -246,12 +246,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>the label for register info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the description </t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -297,9 +291,6 @@
     <t>registry_location</t>
   </si>
   <si>
-    <t>http://registry.it.csiro.au/sandbox/csiro/utils/testreg1</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
     <t>Github repo at  https://github.com/CSIRO-LW-LD/ldrpyutils</t>
   </si>
   <si>
-    <t>Jonathan Yu</t>
-  </si>
-  <si>
     <t>Green book</t>
   </si>
   <si>
@@ -324,13 +312,43 @@
     <t>Yellow book</t>
   </si>
   <si>
-    <t>testreg1</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
     <t>Blue book</t>
+  </si>
+  <si>
+    <t>item5</t>
+  </si>
+  <si>
+    <t>Item 5</t>
+  </si>
+  <si>
+    <t>Description of item 5</t>
+  </si>
+  <si>
+    <t>i5</t>
+  </si>
+  <si>
+    <t>to be noted regarding item 5: this is item 5 which is narrower than 4</t>
+  </si>
+  <si>
+    <t>plucked from thin air</t>
+  </si>
+  <si>
+    <t>testreg4</t>
+  </si>
+  <si>
+    <t>4th test register</t>
+  </si>
+  <si>
+    <t>the description of the 4th test register</t>
+  </si>
+  <si>
+    <t>http://registry.it.csiro.au/sandbox/csiro/utils/testreg4</t>
+  </si>
+  <si>
+    <t>Simon Cox</t>
   </si>
 </sst>
 </file>
@@ -690,7 +708,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,10 +719,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -712,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -720,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -728,31 +746,31 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -767,10 +785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,10 +817,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -810,19 +828,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -830,19 +848,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -853,19 +871,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -876,22 +894,45 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding column with comment in it for altLabel
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\Applications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\git\github\csiro-lw-ld\ldrpyutils\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="registerinfo" sheetId="2" r:id="rId1"/>
     <sheet name="testreg4" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -157,11 +157,24 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
+          <t>An alternate label for the item. Aligned with skos:altLabel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
           <t>A description or definition of the item.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>label</t>
   </si>
@@ -349,6 +362,24 @@
   </si>
   <si>
     <t>Simon Cox</t>
+  </si>
+  <si>
+    <t>altLabel</t>
+  </si>
+  <si>
+    <t>alternative to a</t>
+  </si>
+  <si>
+    <t>alternative to b</t>
+  </si>
+  <si>
+    <t>alternative to c</t>
+  </si>
+  <si>
+    <t>alternative to d</t>
+  </si>
+  <si>
+    <t>alternative to item 5</t>
   </si>
 </sst>
 </file>
@@ -785,22 +816,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -808,22 +840,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -831,19 +866,22 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -851,22 +889,25 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -874,22 +915,25 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -897,7 +941,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -906,13 +950,16 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -920,18 +967,21 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding handling for URLs in broader column
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>label</t>
   </si>
@@ -380,6 +380,21 @@
   </si>
   <si>
     <t>alternative to item 5</t>
+  </si>
+  <si>
+    <t>item 6</t>
+  </si>
+  <si>
+    <t>atl label 6</t>
+  </si>
+  <si>
+    <t>description 6</t>
+  </si>
+  <si>
+    <t>i6</t>
+  </si>
+  <si>
+    <t>http://registry.it.csiro.au/sandbox/csiro/utils/commondef/1</t>
   </si>
 </sst>
 </file>
@@ -816,10 +831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,6 +1000,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing test data for multi reg
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="0" windowWidth="13650" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="1152" yWindow="0" windowWidth="13656" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="registerinfo" sheetId="2" r:id="rId1"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>label</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>http://registry.it.csiro.au/sandbox/csiro/utils/commondef/1</t>
+  </si>
+  <si>
+    <t>notes on description 6</t>
   </si>
 </sst>
 </file>
@@ -754,16 +757,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -771,7 +774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -779,7 +782,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -787,7 +790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -795,7 +798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -803,7 +806,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -811,7 +814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -834,20 +837,20 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="39.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -873,7 +876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -896,7 +899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -922,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -948,7 +951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -974,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1015,6 +1018,9 @@
       </c>
       <c r="E7" t="s">
         <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
       </c>
       <c r="H7" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
adding updated test case file
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\git\github\csiro-lw-ld\ldrpyutils\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\git\github\csiro-env-info\ldrpyutils\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>label</t>
   </si>
@@ -398,6 +398,19 @@
   </si>
   <si>
     <t>notes on description 6</t>
+  </si>
+  <si>
+    <t>multi altLabel</t>
+  </si>
+  <si>
+    <t>altLabel-multi-line1
+altLabel-multi-line2</t>
+  </si>
+  <si>
+    <t>concept with multi alt-labels</t>
+  </si>
+  <si>
+    <t>multi</t>
   </si>
 </sst>
 </file>
@@ -469,10 +482,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -834,16 +850,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="6" max="6" width="39.44140625" customWidth="1"/>
@@ -1026,6 +1043,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix bug with splitting strings unicode
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -403,14 +403,15 @@
     <t>multi altLabel</t>
   </si>
   <si>
+    <t>concept with multi alt-labels</t>
+  </si>
+  <si>
+    <t>multi</t>
+  </si>
+  <si>
     <t>altLabel-multi-line1
-altLabel-multi-line2</t>
-  </si>
-  <si>
-    <t>concept with multi alt-labels</t>
-  </si>
-  <si>
-    <t>multi</t>
+altLabel-multi-line2
+line3</t>
   </si>
 </sst>
 </file>
@@ -853,7 +854,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1044,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1051,13 +1052,13 @@
         <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>54</v>
-      </c>
-      <c r="E8" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding handling for skos relations
</commit_message>
<xml_diff>
--- a/test-data/simple.xlsx
+++ b/test-data/simple.xlsx
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>label</t>
   </si>
@@ -412,6 +412,30 @@
     <t>altLabel-multi-line1
 altLabel-multi-line2
 line3</t>
+  </si>
+  <si>
+    <t>exactMatch</t>
+  </si>
+  <si>
+    <t>test exactMatch</t>
+  </si>
+  <si>
+    <t>closeMatch</t>
+  </si>
+  <si>
+    <t>http://registry.it.csiro.au/def/environment/feature/water-features</t>
+  </si>
+  <si>
+    <t>test closeMatch</t>
+  </si>
+  <si>
+    <t>test related</t>
+  </si>
+  <si>
+    <t>related</t>
+  </si>
+  <si>
+    <t>http://registry.it.csiro.au/def/environment/feature/GroundWaterBody</t>
   </si>
 </sst>
 </file>
@@ -851,10 +875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +892,7 @@
     <col min="7" max="7" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -893,8 +917,17 @@
       <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -917,7 +950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -943,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -969,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -995,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1021,7 +1054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1044,7 +1077,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1059,6 +1092,51 @@
       </c>
       <c r="E8" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>